<commit_message>
Final 2 Project secondary notebook for exporting tables as pngs.
</commit_message>
<xml_diff>
--- a/Exported csv/H4_countries_disc_pref_col_means_sem.xlsx
+++ b/Exported csv/H4_countries_disc_pref_col_means_sem.xlsx
@@ -435,40 +435,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-12123.22113888889</v>
+        <v>-12123.2211</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3980819303874971</v>
+        <v>0.3981</v>
       </c>
       <c r="D2" t="n">
-        <v>-287.5555555555555</v>
+        <v>-287.5556</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4334102524016288</v>
+        <v>0.4334</v>
       </c>
       <c r="F2" t="n">
-        <v>22.23634922339608</v>
+        <v>22.2363</v>
       </c>
       <c r="G2" t="n">
-        <v>25.90739063676666</v>
+        <v>25.9074</v>
       </c>
       <c r="H2" t="n">
-        <v>42020.60852210305</v>
+        <v>42020.6085</v>
       </c>
       <c r="I2" t="n">
-        <v>1488.357771065934</v>
+        <v>1488.3578</v>
       </c>
       <c r="J2" t="n">
-        <v>5.361666666666666</v>
+        <v>5.3617</v>
       </c>
       <c r="K2" t="n">
         <v>5.48</v>
       </c>
       <c r="L2" t="n">
-        <v>1.244700262520653</v>
+        <v>1.2447</v>
       </c>
       <c r="M2" t="n">
-        <v>3.671041413370585</v>
+        <v>3.671</v>
       </c>
     </row>
     <row r="3">
@@ -478,40 +478,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3387.581611011954</v>
+        <v>3387.5816</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02609859283958864</v>
+        <v>0.0261</v>
       </c>
       <c r="D3" t="n">
-        <v>95.43516507807055</v>
+        <v>95.43519999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02849704322596771</v>
+        <v>0.0285</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6437438253369959</v>
+        <v>0.6437</v>
       </c>
       <c r="G3" t="n">
-        <v>1.03791774172182</v>
+        <v>1.0379</v>
       </c>
       <c r="H3" t="n">
-        <v>9675.744055902771</v>
+        <v>9675.7441</v>
       </c>
       <c r="I3" t="n">
-        <v>161.5911868670937</v>
+        <v>161.5912</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9785848292170977</v>
+        <v>0.9786</v>
       </c>
       <c r="K3" t="n">
-        <v>1.282850176428798</v>
+        <v>1.2829</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1352538863742985</v>
+        <v>0.1353</v>
       </c>
       <c r="M3" t="n">
-        <v>1.030677370328055</v>
+        <v>1.0307</v>
       </c>
     </row>
     <row r="4">
@@ -521,40 +521,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14372.29157381641</v>
+        <v>14372.2916</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1107269518577988</v>
+        <v>0.1107</v>
       </c>
       <c r="D4" t="n">
-        <v>404.8971143421676</v>
+        <v>404.8971</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1209027150530876</v>
+        <v>0.1209</v>
       </c>
       <c r="F4" t="n">
-        <v>2.731173745456549</v>
+        <v>2.7312</v>
       </c>
       <c r="G4" t="n">
-        <v>4.403512040911959</v>
+        <v>4.4035</v>
       </c>
       <c r="H4" t="n">
-        <v>41050.70540972567</v>
+        <v>41050.7054</v>
       </c>
       <c r="I4" t="n">
-        <v>685.5733440822272</v>
+        <v>685.5733</v>
       </c>
       <c r="J4" t="n">
-        <v>4.151783812234135</v>
+        <v>4.1518</v>
       </c>
       <c r="K4" t="n">
-        <v>5.442672353994972</v>
+        <v>5.4427</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5738336414226076</v>
+        <v>0.5738</v>
       </c>
       <c r="M4" t="n">
-        <v>4.372793746646916</v>
+        <v>4.3728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>